<commit_message>
enemies now camn only be hit once per turn
</commit_message>
<xml_diff>
--- a/data/info/Part_counts.xlsx
+++ b/data/info/Part_counts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python projects\rogueLike\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python projects\rogueLike\data\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6796FBF6-0B33-45E1-B3CA-EC0EFFB68545}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE87E918-6DC2-47E8-923C-6EB2801D52A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="336" yWindow="960" windowWidth="17280" windowHeight="8964" xr2:uid="{5C234610-992B-44DA-9029-CFA35032CEBB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C234610-992B-44DA-9029-CFA35032CEBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
             <v>partType</v>
           </cell>
           <cell r="E1" t="str">
-            <v>manufactorer</v>
+            <v>manufacturer</v>
           </cell>
         </row>
         <row r="2">
@@ -240,6 +240,54 @@
             <v>guard</v>
           </cell>
           <cell r="E14" t="str">
+            <v>Bright</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="D15" t="str">
+            <v>pommel</v>
+          </cell>
+          <cell r="E15" t="str">
+            <v>Bright</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="D16" t="str">
+            <v>pommel</v>
+          </cell>
+          <cell r="E16" t="str">
+            <v>Bright</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="D17" t="str">
+            <v>handle</v>
+          </cell>
+          <cell r="E17" t="str">
+            <v>Bright</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="D18" t="str">
+            <v>handle</v>
+          </cell>
+          <cell r="E18" t="str">
+            <v>Bright</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="D19" t="str">
+            <v>handle</v>
+          </cell>
+          <cell r="E19" t="str">
+            <v>Bright</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="D20" t="str">
+            <v>handle</v>
+          </cell>
+          <cell r="E20" t="str">
             <v>Bright</v>
           </cell>
         </row>
@@ -549,7 +597,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,7 +689,7 @@
       </c>
       <c r="B4">
         <f>COUNTIFS([1]parts!$E:$E,B$1,[1]parts!$D:$D,$A4)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <f>COUNTIFS([1]parts!$E:$E,C$1,[1]parts!$D:$D,$A4)</f>
@@ -670,7 +718,7 @@
       </c>
       <c r="B5">
         <f>COUNTIFS([1]parts!$E:$E,B$1,[1]parts!$D:$D,$A5)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <f>COUNTIFS([1]parts!$E:$E,C$1,[1]parts!$D:$D,$A5)</f>

</xml_diff>